<commit_message>
working on DI ss
</commit_message>
<xml_diff>
--- a/analyses/pronovo-2020/DI Index for Figure_from_Rick.xlsx
+++ b/analyses/pronovo-2020/DI Index for Figure_from_Rick.xlsx
@@ -5,12 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="lit values" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="our values" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Raw %mol for our samples" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Megan's 2020 peptidomic calcs." sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Megan's 2020 Lee 84 VERTEX calc" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="117">
   <si>
     <t xml:space="preserve">AA</t>
   </si>
@@ -319,6 +321,60 @@
   </si>
   <si>
     <t xml:space="preserve">7 155m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Megan's table: relative molar abundance of suspended particulate amino acids from Table 6 data Lee et al. 1984 VERTEX II Mexico site</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Depth (m)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amino acid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DI 98 coefficient values (static)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thr+Gly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Val</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ala</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Glu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tyr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Orn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lys</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B-ala</t>
   </si>
 </sst>
 </file>
@@ -328,7 +384,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -359,6 +415,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -422,13 +483,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -437,6 +498,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -511,7 +580,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -658,11 +727,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="54456814"/>
-        <c:axId val="96875341"/>
+        <c:axId val="25592257"/>
+        <c:axId val="97398829"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="54456814"/>
+        <c:axId val="25592257"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -728,12 +797,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96875341"/>
+        <c:crossAx val="97398829"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="96875341"/>
+        <c:axId val="97398829"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -799,7 +868,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="54456814"/>
+        <c:crossAx val="25592257"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -831,7 +900,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1117,11 +1186,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="89129774"/>
-        <c:axId val="71889512"/>
+        <c:axId val="37540992"/>
+        <c:axId val="13472464"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="89129774"/>
+        <c:axId val="37540992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1153,12 +1222,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71889512"/>
+        <c:crossAx val="13472464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="71889512"/>
+        <c:axId val="13472464"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1190,7 +1259,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="89129774"/>
+        <c:crossAx val="37540992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1226,16 +1295,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>409680</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>19080</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>153000</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>142920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>552240</xdr:colOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>747360</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>123480</xdr:rowOff>
+      <xdr:rowOff>56160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1243,8 +1312,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="16247160" y="3066840"/>
-        <a:ext cx="5778000" cy="3723840"/>
+        <a:off x="19036440" y="3510720"/>
+        <a:ext cx="5780880" cy="3723480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1259,13 +1328,13 @@
       <xdr:col>14</xdr:col>
       <xdr:colOff>495360</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>57240</xdr:rowOff>
+      <xdr:rowOff>57600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>152280</xdr:colOff>
+      <xdr:colOff>151920</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>152280</xdr:rowOff>
+      <xdr:rowOff>151920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1273,8 +1342,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="14506920" y="5200560"/>
-        <a:ext cx="3759120" cy="4343040"/>
+        <a:off x="14514840" y="5711400"/>
+        <a:ext cx="3760920" cy="4342680"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1295,10 +1364,10 @@
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="1" sqref="A4:K4 B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="20.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="24.57"/>
@@ -1965,13 +2034,13 @@
   </sheetPr>
   <dimension ref="A1:AJ40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="H1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="E30" activeCellId="0" sqref="E30"/>
+      <selection pane="topRight" activeCell="A2" activeCellId="1" sqref="A4:K4 A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.28"/>
@@ -1983,7 +2052,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="66"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="1" customFormat="true" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2100,7 +2169,7 @@
       </c>
       <c r="D2" s="0" t="n">
         <f aca="false">((B2-AF2)/AG2)*$AH2</f>
-        <v>-0.229909447012345</v>
+        <v>-0.229909447012344</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>4.00929255023583</v>
@@ -2111,7 +2180,7 @@
       </c>
       <c r="G2" s="0" t="n">
         <f aca="false">((E2-$AF2)/$AG2)*$AH2</f>
-        <v>0.0513022967647428</v>
+        <v>0.0513022967647431</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>4.46149102820044</v>
@@ -2133,7 +2202,7 @@
       </c>
       <c r="M2" s="0" t="n">
         <f aca="false">((K2-$AF2)/$AG2)*$AH2</f>
-        <v>-0.0430914414612343</v>
+        <v>-0.0430914414612349</v>
       </c>
       <c r="N2" s="0" t="n">
         <v>4.16361642875945</v>
@@ -2144,7 +2213,7 @@
       </c>
       <c r="P2" s="0" t="n">
         <f aca="false">((N2-$AF2)/$AG2)*$AH2</f>
-        <v>6.7291653683653E-005</v>
+        <v>6.72916536839479E-005</v>
       </c>
       <c r="Q2" s="0" t="n">
         <v>4.34255755539816</v>
@@ -2162,11 +2231,11 @@
       </c>
       <c r="U2" s="0" t="n">
         <f aca="false">((T2-7.1)/1.5)*$AH2</f>
-        <v>0.255054298360755</v>
+        <v>0.255054298360754</v>
       </c>
       <c r="V2" s="0" t="n">
         <f aca="false">((T2-$AF2)/$AG2)*$AH2</f>
-        <v>0.00981606815031082</v>
+        <v>0.00981606815030935</v>
       </c>
       <c r="W2" s="0" t="n">
         <v>4.1953873600822</v>
@@ -2177,7 +2246,7 @@
       </c>
       <c r="Y2" s="0" t="n">
         <f aca="false">((W2-$AF2)/$AG2)*$AH2</f>
-        <v>-0.0104805499653614</v>
+        <v>-0.0104805499653629</v>
       </c>
       <c r="Z2" s="0" t="n">
         <v>3.76322724520251</v>
@@ -2188,18 +2257,18 @@
       </c>
       <c r="AB2" s="0" t="n">
         <f aca="false">((Z2-$AF2)/$AG2)*$AH2</f>
-        <v>0.132995144829775</v>
+        <v>0.132995144829774</v>
       </c>
       <c r="AC2" s="0" t="n">
         <v>3.41842820020927</v>
       </c>
       <c r="AD2" s="0" t="n">
         <f aca="false">((AC2-7.1)/1.5)*$AH2</f>
-        <v>0.316615174782002</v>
+        <v>0.316615174782003</v>
       </c>
       <c r="AE2" s="0" t="n">
         <f aca="false">((AC2-$AF2)/$AG2)*$AH2</f>
-        <v>0.247467260237454</v>
+        <v>0.247467260237456</v>
       </c>
       <c r="AF2" s="0" t="n">
         <f aca="false">AVERAGE(B2,E2,H2,K2,N2,Q2,T2,W2,Z2,AC2)</f>
@@ -2207,7 +2276,7 @@
       </c>
       <c r="AG2" s="0" t="n">
         <f aca="false">STDEV(B2,E2,H2,K2,N2,Q2,T2,W2,Z2,AC2)</f>
-        <v>0.388558179830258</v>
+        <v>0.388558179830257</v>
       </c>
       <c r="AH2" s="0" t="n">
         <v>-0.129</v>
@@ -2222,29 +2291,29 @@
       </c>
       <c r="C3" s="0" t="n">
         <f aca="false">((B3-6.1)/2.3)*$AH3</f>
-        <v>-0.10606013851407</v>
+        <v>-0.106060138514071</v>
       </c>
       <c r="D3" s="0" t="n">
         <f aca="false">((B3-AF3)/AG3)*$AH3</f>
-        <v>-0.0790104402858647</v>
+        <v>-0.0790104402858649</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>5.99501640648685</v>
       </c>
       <c r="F3" s="0" t="n">
         <f aca="false">((E3-6.1)/2.3)*$AH3</f>
-        <v>0.00524917967565726</v>
+        <v>0.00524917967565748</v>
       </c>
       <c r="G3" s="0" t="n">
         <f aca="false">((E3-$AF3)/$AG3)*$AH3</f>
-        <v>0.0719977031884504</v>
+        <v>0.0719977031884506</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>9.13589210002509</v>
       </c>
       <c r="I3" s="0" t="n">
         <f aca="false">((H3-6.1)/2.3)*$AH3</f>
-        <v>-0.151794605001254</v>
+        <v>-0.151794605001255</v>
       </c>
       <c r="J3" s="0" t="n">
         <f aca="false">((H3-$AF3)/$AG3)*$AH3</f>
@@ -2277,22 +2346,22 @@
       </c>
       <c r="R3" s="0" t="n">
         <f aca="false">((Q3-6.1)/2.3)*$AH3</f>
-        <v>-0.0838546406313687</v>
+        <v>-0.0838546406313685</v>
       </c>
       <c r="S3" s="0" t="n">
         <f aca="false">((Q3-$AF3)/$AG3)*$AH3</f>
-        <v>-0.0488852803736098</v>
+        <v>-0.0488852803736095</v>
       </c>
       <c r="T3" s="0" t="n">
         <v>5.82828725799647</v>
       </c>
       <c r="U3" s="0" t="n">
         <f aca="false">((T3-6.1)/2.3)*$AH3</f>
-        <v>0.0135856371001764</v>
+        <v>0.0135856371001765</v>
       </c>
       <c r="V3" s="0" t="n">
         <f aca="false">((T3-$AF3)/$AG3)*$AH3</f>
-        <v>0.0833073848871878</v>
+        <v>0.0833073848871879</v>
       </c>
       <c r="W3" s="0" t="n">
         <v>5.30584599603288</v>
@@ -2310,18 +2379,18 @@
       </c>
       <c r="AA3" s="0" t="n">
         <f aca="false">((Z3-6.1)/2.3)*$AH3</f>
-        <v>0.0226238564041973</v>
+        <v>0.0226238564041975</v>
       </c>
       <c r="AB3" s="0" t="n">
         <f aca="false">((Z3-$AF3)/$AG3)*$AH3</f>
-        <v>0.095569114090196</v>
+        <v>0.0955691140901962</v>
       </c>
       <c r="AC3" s="0" t="n">
         <v>5.11722927184498</v>
       </c>
       <c r="AD3" s="0" t="n">
         <f aca="false">((AC3-6.1)/2.3)*$AH3</f>
-        <v>0.0491385364077511</v>
+        <v>0.049138536407751</v>
       </c>
       <c r="AE3" s="0" t="n">
         <f aca="false">((AC3-$AF3)/$AG3)*$AH3</f>
@@ -2348,106 +2417,106 @@
       </c>
       <c r="C4" s="0" t="n">
         <f aca="false">((B4-13.4)/2.7)*$AH4</f>
-        <v>0.0443209297687457</v>
+        <v>0.0443209297687474</v>
       </c>
       <c r="D4" s="0" t="n">
         <f aca="false">((B4-AF4)/AG4)*$AH4</f>
-        <v>0.0704885091642599</v>
+        <v>0.0704885091642638</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>11.0766011593658</v>
       </c>
       <c r="F4" s="0" t="n">
         <f aca="false">((E4-13.4)/2.7)*$AH4</f>
-        <v>0.0877728450906268</v>
+        <v>0.0877728450906253</v>
       </c>
       <c r="G4" s="0" t="n">
         <f aca="false">((E4-$AF4)/$AG4)*$AH4</f>
-        <v>0.171550616797485</v>
+        <v>0.171550616797482</v>
       </c>
       <c r="H4" s="0" t="n">
         <v>13.5024677376123</v>
       </c>
       <c r="I4" s="0" t="n">
         <f aca="false">((H4-13.4)/2.7)*$AH4</f>
-        <v>-0.00387100342090881</v>
+        <v>-0.00387100342090908</v>
       </c>
       <c r="J4" s="0" t="n">
         <f aca="false">((H4-$AF4)/$AG4)*$AH4</f>
-        <v>-0.0415981112525268</v>
+        <v>-0.0415981112525281</v>
       </c>
       <c r="K4" s="0" t="n">
         <v>13.1879332429676</v>
       </c>
       <c r="L4" s="0" t="n">
         <f aca="false">((K4-13.4)/2.7)*$AH4</f>
-        <v>0.00801141082122365</v>
+        <v>0.00801141082122398</v>
       </c>
       <c r="M4" s="0" t="n">
         <f aca="false">((K4-$AF4)/$AG4)*$AH4</f>
-        <v>-0.0139615429175003</v>
+        <v>-0.0139615429174999</v>
       </c>
       <c r="N4" s="0" t="n">
         <v>13.1526458510434</v>
       </c>
       <c r="O4" s="0" t="n">
         <f aca="false">((N4-13.4)/2.7)*$AH4</f>
-        <v>0.00934449007169544</v>
+        <v>0.00934449007169376</v>
       </c>
       <c r="P4" s="0" t="n">
         <f aca="false">((N4-$AF4)/$AG4)*$AH4</f>
-        <v>-0.010861016791165</v>
+        <v>-0.0108610167911693</v>
       </c>
       <c r="Q4" s="0" t="n">
         <v>13.496872132438</v>
       </c>
       <c r="R4" s="0" t="n">
         <f aca="false">((Q4-13.4)/2.7)*$AH4</f>
-        <v>-0.00365961389210167</v>
+        <v>-0.0036596138921022</v>
       </c>
       <c r="S4" s="0" t="n">
         <f aca="false">((Q4-$AF4)/$AG4)*$AH4</f>
-        <v>-0.0411064534934939</v>
+        <v>-0.0411064534934957</v>
       </c>
       <c r="T4" s="0" t="n">
         <v>13.7210251951642</v>
       </c>
       <c r="U4" s="0" t="n">
         <f aca="false">((T4-13.4)/2.7)*$AH4</f>
-        <v>-0.0121276184839817</v>
+        <v>-0.0121276184839809</v>
       </c>
       <c r="V4" s="0" t="n">
         <f aca="false">((T4-$AF4)/$AG4)*$AH4</f>
-        <v>-0.0608016587603667</v>
+        <v>-0.0608016587603655</v>
       </c>
       <c r="W4" s="0" t="n">
         <v>12.4987747029461</v>
       </c>
       <c r="X4" s="0" t="n">
         <f aca="false">((W4-13.4)/2.7)*$AH4</f>
-        <v>0.0340462889998145</v>
+        <v>0.034046288999814</v>
       </c>
       <c r="Y4" s="0" t="n">
         <f aca="false">((W4-$AF4)/$AG4)*$AH4</f>
-        <v>0.046591361165365</v>
+        <v>0.0465913611653637</v>
       </c>
       <c r="Z4" s="0" t="n">
         <v>12.0564882181402</v>
       </c>
       <c r="AA4" s="0" t="n">
         <f aca="false">((Z4-13.4)/2.7)*$AH4</f>
-        <v>0.0507548895369242</v>
+        <v>0.0507548895369258</v>
       </c>
       <c r="AB4" s="0" t="n">
         <f aca="false">((Z4-$AF4)/$AG4)*$AH4</f>
-        <v>0.0854528560700926</v>
+        <v>0.0854528560700964</v>
       </c>
       <c r="AC4" s="0" t="n">
         <v>15.3707483800536</v>
       </c>
       <c r="AD4" s="0" t="n">
         <f aca="false">((AC4-13.4)/2.7)*$AH4</f>
-        <v>-0.0744504943575815</v>
+        <v>-0.0744504943575804</v>
       </c>
       <c r="AE4" s="0" t="n">
         <f aca="false">((AC4-$AF4)/$AG4)*$AH4</f>
@@ -2478,7 +2547,7 @@
       </c>
       <c r="D5" s="0" t="n">
         <f aca="false">((B5-AF5)/AG5)*$AH5</f>
-        <v>0.0746876891258611</v>
+        <v>0.074687689125861</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>8.23604467054269</v>
@@ -2489,7 +2558,7 @@
       </c>
       <c r="G5" s="0" t="n">
         <f aca="false">((E5-$AF5)/$AG5)*$AH5</f>
-        <v>0.106362501781698</v>
+        <v>0.106362501781699</v>
       </c>
       <c r="H5" s="0" t="n">
         <v>10.2008224609531</v>
@@ -2500,18 +2569,18 @@
       </c>
       <c r="J5" s="0" t="n">
         <f aca="false">((H5-$AF5)/$AG5)*$AH5</f>
-        <v>-0.0519966710218487</v>
+        <v>-0.0519966710218476</v>
       </c>
       <c r="K5" s="0" t="n">
         <v>11.6862425608286</v>
       </c>
       <c r="L5" s="0" t="n">
         <f aca="false">((K5-17.6)/3.8)*$AH5</f>
-        <v>0.154068943809991</v>
+        <v>0.154068943809992</v>
       </c>
       <c r="M5" s="0" t="n">
         <f aca="false">((K5-$AF5)/$AG5)*$AH5</f>
-        <v>-0.171720081694618</v>
+        <v>-0.171720081694619</v>
       </c>
       <c r="N5" s="0" t="n">
         <v>10.4648964118611</v>
@@ -2522,18 +2591,18 @@
       </c>
       <c r="P5" s="0" t="n">
         <f aca="false">((N5-$AF5)/$AG5)*$AH5</f>
-        <v>-0.0732807737986908</v>
+        <v>-0.0732807737986913</v>
       </c>
       <c r="Q5" s="0" t="n">
         <v>11.1511334344663</v>
       </c>
       <c r="R5" s="0" t="n">
         <f aca="false">((Q5-17.6)/3.8)*$AH5</f>
-        <v>0.16800994473364</v>
+        <v>0.168009944733641</v>
       </c>
       <c r="S5" s="0" t="n">
         <f aca="false">((Q5-$AF5)/$AG5)*$AH5</f>
-        <v>-0.128590808234815</v>
+        <v>-0.128590808234814</v>
       </c>
       <c r="T5" s="0" t="n">
         <v>8.59984036931811</v>
@@ -2544,14 +2613,14 @@
       </c>
       <c r="V5" s="0" t="n">
         <f aca="false">((T5-$AF5)/$AG5)*$AH5</f>
-        <v>0.0770409234287949</v>
+        <v>0.077040923428795</v>
       </c>
       <c r="W5" s="0" t="n">
         <v>8.4392894301592</v>
       </c>
       <c r="X5" s="0" t="n">
         <f aca="false">((W5-17.6)/3.8)*$AH5</f>
-        <v>0.238660617477432</v>
+        <v>0.238660617477431</v>
       </c>
       <c r="Y5" s="0" t="n">
         <f aca="false">((W5-$AF5)/$AG5)*$AH5</f>
@@ -2566,7 +2635,7 @@
       </c>
       <c r="AB5" s="0" t="n">
         <f aca="false">((Z5-$AF5)/$AG5)*$AH5</f>
-        <v>0.0291565877254995</v>
+        <v>0.0291565877254994</v>
       </c>
       <c r="AC5" s="0" t="n">
         <v>8.95569409673192</v>
@@ -2577,15 +2646,15 @@
       </c>
       <c r="AE5" s="0" t="n">
         <f aca="false">((AC5-$AF5)/$AG5)*$AH5</f>
-        <v>0.0483594602183736</v>
+        <v>0.0483594602183735</v>
       </c>
       <c r="AF5" s="0" t="n">
         <f aca="false">AVERAGE(B5,E5,H5,K5,N5,Q5,T5,W5,Z5,AC5)</f>
-        <v>9.55569466323633</v>
+        <v>9.55569466323632</v>
       </c>
       <c r="AG5" s="0" t="n">
         <f aca="false">STDEV(B5,E5,H5,K5,N5,Q5,T5,W5,Z5,AC5)</f>
-        <v>1.22830271090098</v>
+        <v>1.22830271090097</v>
       </c>
       <c r="AH5" s="0" t="n">
         <v>-0.099</v>
@@ -2600,11 +2669,11 @@
       </c>
       <c r="C6" s="0" t="n">
         <f aca="false">((B6-7.6)/1.1)*$AH6</f>
-        <v>0.0568313959320025</v>
+        <v>0.0568313959320024</v>
       </c>
       <c r="D6" s="0" t="n">
         <f aca="false">((B6-AF6)/AG6)*$AH6</f>
-        <v>-0.0824890324043524</v>
+        <v>-0.0824890324043526</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>4.88336951876439</v>
@@ -2626,29 +2695,29 @@
       </c>
       <c r="J6" s="0" t="n">
         <f aca="false">((H6-$AF6)/$AG6)*$AH6</f>
-        <v>0.00325144263263227</v>
+        <v>0.00325144263263255</v>
       </c>
       <c r="K6" s="0" t="n">
         <v>4.22972548861579</v>
       </c>
       <c r="L6" s="0" t="n">
         <f aca="false">((K6-7.6)/1.1)*$AH6</f>
-        <v>0.134810980455369</v>
+        <v>0.134810980455368</v>
       </c>
       <c r="M6" s="0" t="n">
         <f aca="false">((K6-$AF6)/$AG6)*$AH6</f>
-        <v>0.0414119264215894</v>
+        <v>0.0414119264215891</v>
       </c>
       <c r="N6" s="0" t="n">
         <v>5.12173294424539</v>
       </c>
       <c r="O6" s="0" t="n">
         <f aca="false">((N6-7.6)/1.1)*$AH6</f>
-        <v>0.0991306822301842</v>
+        <v>0.0991306822301844</v>
       </c>
       <c r="P6" s="0" t="n">
         <f aca="false">((N6-$AF6)/$AG6)*$AH6</f>
-        <v>-0.0152801319975116</v>
+        <v>-0.0152801319975113</v>
       </c>
       <c r="Q6" s="0" t="n">
         <v>4.34159520112607</v>
@@ -2659,29 +2728,29 @@
       </c>
       <c r="S6" s="0" t="n">
         <f aca="false">((Q6-$AF6)/$AG6)*$AH6</f>
-        <v>0.034301981054054</v>
+        <v>0.0343019810540536</v>
       </c>
       <c r="T6" s="0" t="n">
         <v>5.30584354895344</v>
       </c>
       <c r="U6" s="0" t="n">
         <f aca="false">((T6-7.6)/1.1)*$AH6</f>
-        <v>0.0917662580418626</v>
+        <v>0.0917662580418624</v>
       </c>
       <c r="V6" s="0" t="n">
         <f aca="false">((T6-$AF6)/$AG6)*$AH6</f>
-        <v>-0.0269813897524897</v>
+        <v>-0.02698138975249</v>
       </c>
       <c r="W6" s="0" t="n">
         <v>5.38153797504682</v>
       </c>
       <c r="X6" s="0" t="n">
         <f aca="false">((W6-7.6)/1.1)*$AH6</f>
-        <v>0.088738480998127</v>
+        <v>0.0887384809981272</v>
       </c>
       <c r="Y6" s="0" t="n">
         <f aca="false">((W6-$AF6)/$AG6)*$AH6</f>
-        <v>-0.0317921935176418</v>
+        <v>-0.0317921935176416</v>
       </c>
       <c r="Z6" s="0" t="n">
         <v>4.85084998526936</v>
@@ -2692,7 +2761,7 @@
       </c>
       <c r="AB6" s="0" t="n">
         <f aca="false">((Z6-$AF6)/$AG6)*$AH6</f>
-        <v>0.00193599376252373</v>
+        <v>0.00193599376252356</v>
       </c>
       <c r="AC6" s="0" t="n">
         <v>3.68909196247403</v>
@@ -2703,7 +2772,7 @@
       </c>
       <c r="AE6" s="0" t="n">
         <f aca="false">((AC6-$AF6)/$AG6)*$AH6</f>
-        <v>0.0757722081142119</v>
+        <v>0.075772208114212</v>
       </c>
       <c r="AF6" s="0" t="n">
         <f aca="false">AVERAGE(B6,E6,H6,K6,N6,Q6,T6,W6,Z6,AC6)</f>
@@ -2726,11 +2795,11 @@
       </c>
       <c r="C7" s="0" t="n">
         <f aca="false">((B7-11.8)/0.8)*$AH7</f>
-        <v>0.0713080143980925</v>
+        <v>0.0713080143980943</v>
       </c>
       <c r="D7" s="0" t="n">
         <f aca="false">((B7-AF7)/AG7)*$AH7</f>
-        <v>-0.043247739907448</v>
+        <v>-0.0432477399074472</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>7.24235023857234</v>
@@ -2741,7 +2810,7 @@
       </c>
       <c r="G7" s="0" t="n">
         <f aca="false">((E7-$AF7)/$AG7)*$AH7</f>
-        <v>0.032721012738674</v>
+        <v>0.0327210127386741</v>
       </c>
       <c r="H7" s="0" t="n">
         <v>8.66472535867728</v>
@@ -2759,11 +2828,11 @@
       </c>
       <c r="L7" s="0" t="n">
         <f aca="false">((K7-11.8)/0.8)*$AH7</f>
-        <v>-0.000845688386647323</v>
+        <v>-0.000845688386647418</v>
       </c>
       <c r="M7" s="0" t="n">
         <f aca="false">((K7-$AF7)/$AG7)*$AH7</f>
-        <v>-0.0748108410442002</v>
+        <v>-0.0748108410442003</v>
       </c>
       <c r="N7" s="0" t="n">
         <v>9.08327960985352</v>
@@ -2781,11 +2850,11 @@
       </c>
       <c r="R7" s="0" t="n">
         <f aca="false">((Q7-11.8)/0.8)*$AH7</f>
-        <v>0.0826534079739432</v>
+        <v>0.0826534079739413</v>
       </c>
       <c r="S7" s="0" t="n">
         <f aca="false">((Q7-$AF7)/$AG7)*$AH7</f>
-        <v>-0.038284781790951</v>
+        <v>-0.0382847817909518</v>
       </c>
       <c r="T7" s="0" t="n">
         <v>6.10259737280117</v>
@@ -2807,7 +2876,7 @@
       </c>
       <c r="Y7" s="0" t="n">
         <f aca="false">((W7-$AF7)/$AG7)*$AH7</f>
-        <v>0.0225041557632138</v>
+        <v>0.0225041557632137</v>
       </c>
       <c r="Z7" s="0" t="n">
         <v>6.52195489090845</v>
@@ -2829,7 +2898,7 @@
       </c>
       <c r="AE7" s="0" t="n">
         <f aca="false">((AC7-$AF7)/$AG7)*$AH7</f>
-        <v>0.00322590873778108</v>
+        <v>0.00322590873778104</v>
       </c>
       <c r="AF7" s="0" t="n">
         <f aca="false">AVERAGE(B7,E7,H7,K7,N7,Q7,T7,W7,Z7,AC7)</f>
@@ -2853,51 +2922,51 @@
       </c>
       <c r="C8" s="0" t="n">
         <f aca="false">((B8-7.2)/1.9)*$AH8</f>
-        <v>-0.00673147761691004</v>
+        <v>-0.00673147761691003</v>
       </c>
       <c r="D8" s="0" t="n">
         <f aca="false">((B8-AF8)/AG8)*$AH8</f>
-        <v>0.000553270933738449</v>
+        <v>0.000553270933738462</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>5.69776713482597</v>
       </c>
       <c r="F8" s="0" t="n">
         <f aca="false">((E8-7.2)/1.9)*$AH8</f>
-        <v>-0.0118597331461107</v>
+        <v>-0.0118597331461108</v>
       </c>
       <c r="G8" s="0" t="n">
         <f aca="false">((E8-$AF8)/$AG8)*$AH8</f>
-        <v>-0.00836065925942463</v>
+        <v>-0.00836065925942471</v>
       </c>
       <c r="H8" s="0" t="n">
         <v>6.63122801578761</v>
       </c>
       <c r="I8" s="0" t="n">
         <f aca="false">((H8-7.2)/1.9)*$AH8</f>
-        <v>-0.00449030513851891</v>
+        <v>-0.00449030513851887</v>
       </c>
       <c r="J8" s="0" t="n">
         <f aca="false">((H8-$AF8)/$AG8)*$AH8</f>
-        <v>0.004448875376509</v>
+        <v>0.00444887537650905</v>
       </c>
       <c r="K8" s="0" t="n">
         <v>8.33264920468809</v>
       </c>
       <c r="L8" s="0" t="n">
         <f aca="false">((K8-7.2)/1.9)*$AH8</f>
-        <v>0.00894196740543232</v>
+        <v>0.00894196740543229</v>
       </c>
       <c r="M8" s="0" t="n">
         <f aca="false">((K8-$AF8)/$AG8)*$AH8</f>
-        <v>0.0277968421676616</v>
+        <v>0.0277968421676615</v>
       </c>
       <c r="N8" s="0" t="n">
         <v>6.48556217545495</v>
       </c>
       <c r="O8" s="0" t="n">
         <f aca="false">((N8-7.2)/1.9)*$AH8</f>
-        <v>-0.00564029861482935</v>
+        <v>-0.00564029861482934</v>
       </c>
       <c r="P8" s="0" t="n">
         <f aca="false">((N8-$AF8)/$AG8)*$AH8</f>
@@ -2908,7 +2977,7 @@
       </c>
       <c r="R8" s="0" t="n">
         <f aca="false">((Q8-7.2)/1.9)*$AH8</f>
-        <v>0.00328435396649639</v>
+        <v>0.00328435396649637</v>
       </c>
       <c r="S8" s="0" t="n">
         <f aca="false">((Q8-$AF8)/$AG8)*$AH8</f>
@@ -2941,22 +3010,22 @@
       </c>
       <c r="AA8" s="0" t="n">
         <f aca="false">((Z8-7.2)/1.9)*$AH8</f>
-        <v>-0.0112849353193942</v>
+        <v>-0.0112849353193941</v>
       </c>
       <c r="AB8" s="0" t="n">
         <f aca="false">((Z8-$AF8)/$AG8)*$AH8</f>
-        <v>-0.00736154607690895</v>
+        <v>-0.00736154607690892</v>
       </c>
       <c r="AC8" s="0" t="n">
         <v>6.383248123109</v>
       </c>
       <c r="AD8" s="0" t="n">
         <f aca="false">((AC8-7.2)/1.9)*$AH8</f>
-        <v>-0.00644804113334998</v>
+        <v>-0.00644804113335</v>
       </c>
       <c r="AE8" s="0" t="n">
         <f aca="false">((AC8-$AF8)/$AG8)*$AH8</f>
-        <v>0.00104594003227765</v>
+        <v>0.00104594003227761</v>
       </c>
       <c r="AF8" s="0" t="n">
         <f aca="false">AVERAGE(B8,E8,H8,K8,N8,Q8,T8,W8,Z8,AC8)</f>
@@ -2979,44 +3048,44 @@
       </c>
       <c r="C9" s="0" t="n">
         <f aca="false">((B9-10)/2.3)*$AH9</f>
-        <v>0.0165256478803334</v>
+        <v>0.0165256478803339</v>
       </c>
       <c r="D9" s="0" t="n">
         <f aca="false">((B9-AF9)/AG9)*$AH9</f>
-        <v>-0.0725922579129339</v>
+        <v>-0.0725922579129335</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>11.0341607402404</v>
       </c>
       <c r="F9" s="0" t="n">
         <f aca="false">((E9-10)/2.3)*$AH9</f>
-        <v>0.0292262817894028</v>
+        <v>0.0292262817894026</v>
       </c>
       <c r="G9" s="0" t="n">
         <f aca="false">((E9-$AF9)/$AG9)*$AH9</f>
-        <v>-0.0564970026774558</v>
+        <v>-0.0564970026774561</v>
       </c>
       <c r="H9" s="0" t="n">
         <v>14.9472854855419</v>
       </c>
       <c r="I9" s="0" t="n">
         <f aca="false">((H9-10)/2.3)*$AH9</f>
-        <v>0.139814589808794</v>
+        <v>0.139814589808793</v>
       </c>
       <c r="J9" s="0" t="n">
         <f aca="false">((H9-$AF9)/$AG9)*$AH9</f>
-        <v>0.0836493125675444</v>
+        <v>0.0836493125675436</v>
       </c>
       <c r="K9" s="0" t="n">
         <v>13.964582261204</v>
       </c>
       <c r="L9" s="0" t="n">
         <f aca="false">((K9-10)/2.3)*$AH9</f>
-        <v>0.112042542164462</v>
+        <v>0.112042542164461</v>
       </c>
       <c r="M9" s="0" t="n">
         <f aca="false">((K9-$AF9)/$AG9)*$AH9</f>
-        <v>0.0484543610046796</v>
+        <v>0.048454361004678</v>
       </c>
       <c r="N9" s="0" t="n">
         <v>14.6510375825993</v>
@@ -3027,62 +3096,62 @@
       </c>
       <c r="P9" s="0" t="n">
         <f aca="false">((N9-$AF9)/$AG9)*$AH9</f>
-        <v>0.0730393640739989</v>
+        <v>0.073039364073999</v>
       </c>
       <c r="Q9" s="0" t="n">
         <v>14.9749889486229</v>
       </c>
       <c r="R9" s="0" t="n">
         <f aca="false">((Q9-10)/2.3)*$AH9</f>
-        <v>0.140597513765428</v>
+        <v>0.14059751376543</v>
       </c>
       <c r="S9" s="0" t="n">
         <f aca="false">((Q9-$AF9)/$AG9)*$AH9</f>
-        <v>0.08464149618627</v>
+        <v>0.0846414961862717</v>
       </c>
       <c r="T9" s="0" t="n">
         <v>12.3170338073268</v>
       </c>
       <c r="U9" s="0" t="n">
         <f aca="false">((T9-10)/2.3)*$AH9</f>
-        <v>0.0654813902070606</v>
+        <v>0.0654813902070617</v>
       </c>
       <c r="V9" s="0" t="n">
         <f aca="false">((T9-$AF9)/$AG9)*$AH9</f>
-        <v>-0.01055164059947</v>
+        <v>-0.0105516405994686</v>
       </c>
       <c r="W9" s="0" t="n">
         <v>11.0435018540618</v>
       </c>
       <c r="X9" s="0" t="n">
         <f aca="false">((W9-10)/2.3)*$AH9</f>
-        <v>0.0294902697887031</v>
+        <v>0.029490269788703</v>
       </c>
       <c r="Y9" s="0" t="n">
         <f aca="false">((W9-$AF9)/$AG9)*$AH9</f>
-        <v>-0.0561624560510226</v>
+        <v>-0.0561624560510228</v>
       </c>
       <c r="Z9" s="0" t="n">
         <v>11.4208213945066</v>
       </c>
       <c r="AA9" s="0" t="n">
         <f aca="false">((Z9-10)/2.3)*$AH9</f>
-        <v>0.0401536481056204</v>
+        <v>0.0401536481056213</v>
       </c>
       <c r="AB9" s="0" t="n">
         <f aca="false">((Z9-$AF9)/$AG9)*$AH9</f>
-        <v>-0.0426489734239319</v>
+        <v>-0.0426489734239309</v>
       </c>
       <c r="AC9" s="0" t="n">
         <v>11.1783707733825</v>
       </c>
       <c r="AD9" s="0" t="n">
         <f aca="false">((AC9-10)/2.3)*$AH9</f>
-        <v>0.033301782726028</v>
+        <v>0.0333017827260272</v>
       </c>
       <c r="AE9" s="0" t="n">
         <f aca="false">((AC9-$AF9)/$AG9)*$AH9</f>
-        <v>-0.0513322031676791</v>
+        <v>-0.0513322031676803</v>
       </c>
       <c r="AF9" s="0" t="n">
         <f aca="false">AVERAGE(B9,E9,H9,K9,N9,Q9,T9,W9,Z9,AC9)</f>
@@ -3109,18 +3178,18 @@
       </c>
       <c r="D10" s="0" t="n">
         <f aca="false">((B10-AF10)/AG10)*$AH10</f>
-        <v>0.210919963973728</v>
+        <v>0.210919963973729</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>3.25325308958636</v>
       </c>
       <c r="F10" s="0" t="n">
         <f aca="false">((E10-1.2)/1)*$AH10</f>
-        <v>0.275135914004573</v>
+        <v>0.275135914004572</v>
       </c>
       <c r="G10" s="0" t="n">
         <f aca="false">((E10-$AF10)/$AG10)*$AH10</f>
-        <v>0.0783036813910548</v>
+        <v>0.0783036813910537</v>
       </c>
       <c r="H10" s="0" t="n">
         <v>2.60360069549101</v>
@@ -3131,18 +3200,18 @@
       </c>
       <c r="J10" s="0" t="n">
         <f aca="false">((H10-$AF10)/$AG10)*$AH10</f>
-        <v>-0.0863633287798621</v>
+        <v>-0.0863633287798619</v>
       </c>
       <c r="K10" s="0" t="n">
         <v>2.50822833280679</v>
       </c>
       <c r="L10" s="0" t="n">
         <f aca="false">((K10-1.2)/1)*$AH10</f>
-        <v>0.175302596596109</v>
+        <v>0.17530259659611</v>
       </c>
       <c r="M10" s="0" t="n">
         <f aca="false">((K10-$AF10)/$AG10)*$AH10</f>
-        <v>-0.110537305446286</v>
+        <v>-0.110537305446285</v>
       </c>
       <c r="N10" s="0" t="n">
         <v>3.13561246715465</v>
@@ -3153,18 +3222,18 @@
       </c>
       <c r="P10" s="0" t="n">
         <f aca="false">((N10-$AF10)/$AG10)*$AH10</f>
-        <v>0.0484853820258209</v>
+        <v>0.0484853820258211</v>
       </c>
       <c r="Q10" s="0" t="n">
         <v>2.12418768996495</v>
       </c>
       <c r="R10" s="0" t="n">
         <f aca="false">((Q10-1.2)/1)*$AH10</f>
-        <v>0.123841150455304</v>
+        <v>0.123841150455303</v>
       </c>
       <c r="S10" s="0" t="n">
         <f aca="false">((Q10-$AF10)/$AG10)*$AH10</f>
-        <v>-0.207879861274071</v>
+        <v>-0.207879861274072</v>
       </c>
       <c r="T10" s="0" t="n">
         <v>3.49192254526896</v>
@@ -3175,7 +3244,7 @@
       </c>
       <c r="V10" s="0" t="n">
         <f aca="false">((T10-$AF10)/$AG10)*$AH10</f>
-        <v>0.13879908792473</v>
+        <v>0.138799087924729</v>
       </c>
       <c r="W10" s="0" t="n">
         <v>3.27202219604798</v>
@@ -3186,18 +3255,18 @@
       </c>
       <c r="Y10" s="0" t="n">
         <f aca="false">((W10-$AF10)/$AG10)*$AH10</f>
-        <v>0.0830610757648832</v>
+        <v>0.0830610757648839</v>
       </c>
       <c r="Z10" s="0" t="n">
         <v>2.88217447320299</v>
       </c>
       <c r="AA10" s="0" t="n">
         <f aca="false">((Z10-1.2)/1)*$AH10</f>
-        <v>0.2254113794092</v>
+        <v>0.225411379409201</v>
       </c>
       <c r="AB10" s="0" t="n">
         <f aca="false">((Z10-$AF10)/$AG10)*$AH10</f>
-        <v>-0.0157533972152663</v>
+        <v>-0.0157533972152653</v>
       </c>
       <c r="AC10" s="0" t="n">
         <v>2.3957966483597</v>
@@ -3208,7 +3277,7 @@
       </c>
       <c r="AE10" s="0" t="n">
         <f aca="false">((AC10-$AF10)/$AG10)*$AH10</f>
-        <v>-0.139035298364732</v>
+        <v>-0.139035298364733</v>
       </c>
       <c r="AF10" s="0" t="n">
         <f aca="false">AVERAGE(B10,E10,H10,K10,N10,Q10,T10,W10,Z10,AC10)</f>
@@ -3216,7 +3285,7 @@
       </c>
       <c r="AG10" s="0" t="n">
         <f aca="false">STDEV(B10,E10,H10,K10,N10,Q10,T10,W10,Z10,AC10)</f>
-        <v>0.528663396016118</v>
+        <v>0.528663396016119</v>
       </c>
       <c r="AH10" s="0" t="n">
         <v>0.134</v>
@@ -3232,22 +3301,22 @@
       </c>
       <c r="C11" s="0" t="n">
         <f aca="false">((B11-3.7)/1.2)*$AH11</f>
-        <v>0.317446644992321</v>
+        <v>0.31744664499232</v>
       </c>
       <c r="D11" s="0" t="n">
         <f aca="false">((B11-AF11)/AG11)*$AH11</f>
-        <v>0.118230407224727</v>
+        <v>0.118230407224726</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>5.52738527073233</v>
       </c>
       <c r="F11" s="0" t="n">
         <f aca="false">((E11-3.7)/1.2)*$AH11</f>
-        <v>0.204058021898444</v>
+        <v>0.204058021898443</v>
       </c>
       <c r="G11" s="0" t="n">
         <f aca="false">((E11-$AF11)/$AG11)*$AH11</f>
-        <v>-0.0576517873582083</v>
+        <v>-0.0576517873582086</v>
       </c>
       <c r="H11" s="0" t="n">
         <v>6.78697149437664</v>
@@ -3258,7 +3327,7 @@
       </c>
       <c r="J11" s="0" t="n">
         <f aca="false">((H11-$AF11)/$AG11)*$AH11</f>
-        <v>0.160522641974935</v>
+        <v>0.160522641974936</v>
       </c>
       <c r="K11" s="0" t="n">
         <v>6.72543003866058</v>
@@ -3280,14 +3349,14 @@
       </c>
       <c r="P11" s="0" t="n">
         <f aca="false">((N11-$AF11)/$AG11)*$AH11</f>
-        <v>0.0372825671327802</v>
+        <v>0.0372825671327806</v>
       </c>
       <c r="Q11" s="0" t="n">
         <v>6.45356513990221</v>
       </c>
       <c r="R11" s="0" t="n">
         <f aca="false">((Q11-3.7)/1.2)*$AH11</f>
-        <v>0.307481440622414</v>
+        <v>0.307481440622413</v>
       </c>
       <c r="S11" s="0" t="n">
         <f aca="false">((Q11-$AF11)/$AG11)*$AH11</f>
@@ -3309,11 +3378,11 @@
       </c>
       <c r="X11" s="0" t="n">
         <f aca="false">((W11-3.7)/1.2)*$AH11</f>
-        <v>0.210729222637686</v>
+        <v>0.210729222637687</v>
       </c>
       <c r="Y11" s="0" t="n">
         <f aca="false">((W11-$AF11)/$AG11)*$AH11</f>
-        <v>-0.0473037877573149</v>
+        <v>-0.0473037877573137</v>
       </c>
       <c r="Z11" s="0" t="n">
         <v>5.30672404794614</v>
@@ -3324,14 +3393,14 @@
       </c>
       <c r="AB11" s="0" t="n">
         <f aca="false">((Z11-$AF11)/$AG11)*$AH11</f>
-        <v>-0.095872780453895</v>
+        <v>-0.0958727804538948</v>
       </c>
       <c r="AC11" s="0" t="n">
         <v>4.50858580845123</v>
       </c>
       <c r="AD11" s="0" t="n">
         <f aca="false">((AC11-3.7)/1.2)*$AH11</f>
-        <v>0.090292081943721</v>
+        <v>0.0902920819437206</v>
       </c>
       <c r="AE11" s="0" t="n">
         <f aca="false">((AC11-$AF11)/$AG11)*$AH11</f>
@@ -3343,7 +3412,7 @@
       </c>
       <c r="AG11" s="0" t="n">
         <f aca="false">STDEV(B11,E11,H11,K11,N11,Q11,T11,W11,Z11,AC11)</f>
-        <v>0.773622071496791</v>
+        <v>0.773622071496793</v>
       </c>
       <c r="AH11" s="0" t="n">
         <v>0.134</v>
@@ -3358,44 +3427,44 @@
       </c>
       <c r="C12" s="0" t="n">
         <f aca="false">((B12-4.5)/0.8)*$AH12</f>
-        <v>-0.113404953344075</v>
+        <v>-0.113404953344074</v>
       </c>
       <c r="D12" s="0" t="n">
         <f aca="false">((B12-AF12)/AG12)*$AH12</f>
-        <v>0.171133669362805</v>
+        <v>0.171133669362806</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>3.27909909658547</v>
       </c>
       <c r="F12" s="0" t="n">
         <f aca="false">((E12-4.5)/0.8)*$AH12</f>
-        <v>-0.212131531968274</v>
+        <v>-0.212131531968275</v>
       </c>
       <c r="G12" s="0" t="n">
         <f aca="false">((E12-$AF12)/$AG12)*$AH12</f>
-        <v>0.0423130545922039</v>
+        <v>0.0423130545922035</v>
       </c>
       <c r="H12" s="0" t="n">
         <v>2.79349279109419</v>
       </c>
       <c r="I12" s="0" t="n">
         <f aca="false">((H12-4.5)/0.8)*$AH12</f>
-        <v>-0.296505627547384</v>
+        <v>-0.296505627547385</v>
       </c>
       <c r="J12" s="0" t="n">
         <f aca="false">((H12-$AF12)/$AG12)*$AH12</f>
-        <v>-0.0677801241108417</v>
+        <v>-0.067780124110843</v>
       </c>
       <c r="K12" s="0" t="n">
         <v>2.10892940659486</v>
       </c>
       <c r="L12" s="0" t="n">
         <f aca="false">((K12-4.5)/0.8)*$AH12</f>
-        <v>-0.415448515604144</v>
+        <v>-0.415448515604143</v>
       </c>
       <c r="M12" s="0" t="n">
         <f aca="false">((K12-$AF12)/$AG12)*$AH12</f>
-        <v>-0.222979424801556</v>
+        <v>-0.222979424801555</v>
       </c>
       <c r="N12" s="0" t="n">
         <v>3.19227342731554</v>
@@ -3413,29 +3482,29 @@
       </c>
       <c r="R12" s="0" t="n">
         <f aca="false">((Q12-4.5)/0.8)*$AH12</f>
-        <v>-0.366430782146037</v>
+        <v>-0.366430782146036</v>
       </c>
       <c r="S12" s="0" t="n">
         <f aca="false">((Q12-$AF12)/$AG12)*$AH12</f>
-        <v>-0.159020006307264</v>
+        <v>-0.159020006307263</v>
       </c>
       <c r="T12" s="0" t="n">
         <v>3.86734047736486</v>
       </c>
       <c r="U12" s="0" t="n">
         <f aca="false">((T12-4.5)/0.8)*$AH12</f>
-        <v>-0.109924592057855</v>
+        <v>-0.109924592057856</v>
       </c>
       <c r="V12" s="0" t="n">
         <f aca="false">((T12-$AF12)/$AG12)*$AH12</f>
-        <v>0.175674921442665</v>
+        <v>0.175674921442664</v>
       </c>
       <c r="W12" s="0" t="n">
         <v>3.72193194999819</v>
       </c>
       <c r="X12" s="0" t="n">
         <f aca="false">((W12-4.5)/0.8)*$AH12</f>
-        <v>-0.135189323687815</v>
+        <v>-0.135189323687814</v>
       </c>
       <c r="Y12" s="0" t="n">
         <f aca="false">((W12-$AF12)/$AG12)*$AH12</f>
@@ -3450,7 +3519,7 @@
       </c>
       <c r="AB12" s="0" t="n">
         <f aca="false">((Z12-$AF12)/$AG12)*$AH12</f>
-        <v>0.00239620575871017</v>
+        <v>0.00239620575870966</v>
       </c>
       <c r="AC12" s="0" t="n">
         <v>2.62016481128346</v>
@@ -3488,7 +3557,7 @@
       </c>
       <c r="D13" s="0" t="n">
         <f aca="false">((B13-AF13)/AG13)*$AH13</f>
-        <v>0.14831382029371</v>
+        <v>0.148313820293711</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>1.9735376633002</v>
@@ -3499,7 +3568,7 @@
       </c>
       <c r="G13" s="0" t="n">
         <f aca="false">((E13-$AF13)/$AG13)*$AH13</f>
-        <v>-0.0369049017110386</v>
+        <v>-0.0369049017110391</v>
       </c>
       <c r="H13" s="0" t="n">
         <v>1.25174639610995</v>
@@ -3517,11 +3586,11 @@
       </c>
       <c r="L13" s="0" t="n">
         <f aca="false">((K13-1)/0.8)*$AH13</f>
-        <v>0.0985916414572037</v>
+        <v>0.0985916414572044</v>
       </c>
       <c r="M13" s="0" t="n">
         <f aca="false">((K13-$AF13)/$AG13)*$AH13</f>
-        <v>-0.162032154111046</v>
+        <v>-0.162032154111045</v>
       </c>
       <c r="N13" s="0" t="n">
         <v>2.10019785524528</v>
@@ -3532,36 +3601,36 @@
       </c>
       <c r="P13" s="0" t="n">
         <f aca="false">((N13-$AF13)/$AG13)*$AH13</f>
-        <v>-0.00349287821732701</v>
+        <v>-0.00349287821732738</v>
       </c>
       <c r="Q13" s="0" t="n">
         <v>2.43168464605448</v>
       </c>
       <c r="R13" s="0" t="n">
         <f aca="false">((Q13-1)/0.8)*$AH13</f>
-        <v>0.282757717595761</v>
+        <v>0.28275771759576</v>
       </c>
       <c r="S13" s="0" t="n">
         <f aca="false">((Q13-$AF13)/$AG13)*$AH13</f>
-        <v>0.0839508898070771</v>
+        <v>0.0839508898070768</v>
       </c>
       <c r="T13" s="0" t="n">
         <v>2.07399489370266</v>
       </c>
       <c r="U13" s="0" t="n">
         <f aca="false">((T13-1)/0.8)*$AH13</f>
-        <v>0.212113991506276</v>
+        <v>0.212113991506275</v>
       </c>
       <c r="V13" s="0" t="n">
         <f aca="false">((T13-$AF13)/$AG13)*$AH13</f>
-        <v>-0.0104050260139016</v>
+        <v>-0.0104050260139015</v>
       </c>
       <c r="W13" s="0" t="n">
         <v>3.36357957874017</v>
       </c>
       <c r="X13" s="0" t="n">
         <f aca="false">((W13-1)/0.8)*$AH13</f>
-        <v>0.466806966801185</v>
+        <v>0.466806966801184</v>
       </c>
       <c r="Y13" s="0" t="n">
         <f aca="false">((W13-$AF13)/$AG13)*$AH13</f>
@@ -3576,18 +3645,18 @@
       </c>
       <c r="AB13" s="0" t="n">
         <f aca="false">((Z13-$AF13)/$AG13)*$AH13</f>
-        <v>-0.065544337080223</v>
+        <v>-0.0655443370802226</v>
       </c>
       <c r="AC13" s="0" t="n">
         <v>1.89980438249092</v>
       </c>
       <c r="AD13" s="0" t="n">
         <f aca="false">((AC13-1)/0.8)*$AH13</f>
-        <v>0.177711365541958</v>
+        <v>0.177711365541957</v>
       </c>
       <c r="AE13" s="0" t="n">
         <f aca="false">((AC13-$AF13)/$AG13)*$AH13</f>
-        <v>-0.0563551968103566</v>
+        <v>-0.0563551968103574</v>
       </c>
       <c r="AF13" s="0" t="n">
         <f aca="false">AVERAGE(B13,E13,H13,K13,N13,Q13,T13,W13,Z13,AC13)</f>
@@ -3595,7 +3664,7 @@
       </c>
       <c r="AG13" s="0" t="n">
         <f aca="false">STDEV(B13,E13,H13,K13,N13,Q13,T13,W13,Z13,AC13)</f>
-        <v>0.598955353035984</v>
+        <v>0.598955353035983</v>
       </c>
       <c r="AH13" s="0" t="n">
         <v>0.158</v>
@@ -3610,7 +3679,7 @@
       </c>
       <c r="C14" s="0" t="n">
         <f aca="false">((B14-6.6)/1.5)*$AH14</f>
-        <v>0.0564540272571062</v>
+        <v>0.0564540272571065</v>
       </c>
       <c r="D14" s="0" t="n">
         <f aca="false">((B14-AF14)/AG14)*$AH14</f>
@@ -3621,44 +3690,44 @@
       </c>
       <c r="F14" s="0" t="n">
         <f aca="false">((E14-6.6)/1.5)*$AH14</f>
-        <v>0.0205866345001789</v>
+        <v>0.0205866345001785</v>
       </c>
       <c r="G14" s="0" t="n">
         <f aca="false">((E14-$AF14)/$AG14)*$AH14</f>
-        <v>0.139240727817142</v>
+        <v>0.139240727817141</v>
       </c>
       <c r="H14" s="0" t="n">
         <v>5.9373332324765</v>
       </c>
       <c r="I14" s="0" t="n">
         <f aca="false">((H14-6.6)/1.5)*$AH14</f>
-        <v>-0.0746604558076481</v>
+        <v>-0.0746604558076476</v>
       </c>
       <c r="J14" s="0" t="n">
         <f aca="false">((H14-$AF14)/$AG14)*$AH14</f>
-        <v>-0.0868116210117288</v>
+        <v>-0.0868116210117283</v>
       </c>
       <c r="K14" s="0" t="n">
         <v>5.80536439676304</v>
       </c>
       <c r="L14" s="0" t="n">
         <f aca="false">((K14-6.6)/1.5)*$AH14</f>
-        <v>-0.0895289446313643</v>
+        <v>-0.0895289446313641</v>
       </c>
       <c r="M14" s="0" t="n">
         <f aca="false">((K14-$AF14)/$AG14)*$AH14</f>
-        <v>-0.12209938477726</v>
+        <v>-0.122099384777261</v>
       </c>
       <c r="N14" s="0" t="n">
         <v>6.03173212377946</v>
       </c>
       <c r="O14" s="0" t="n">
         <f aca="false">((N14-6.6)/1.5)*$AH14</f>
-        <v>-0.0640248473875147</v>
+        <v>-0.0640248473875141</v>
       </c>
       <c r="P14" s="0" t="n">
         <f aca="false">((N14-$AF14)/$AG14)*$AH14</f>
-        <v>-0.0615698602731574</v>
+        <v>-0.0615698602731565</v>
       </c>
       <c r="Q14" s="0" t="n">
         <v>5.31383567550206</v>
@@ -3669,25 +3738,25 @@
       </c>
       <c r="S14" s="0" t="n">
         <f aca="false">((Q14-$AF14)/$AG14)*$AH14</f>
-        <v>-0.253531546818094</v>
+        <v>-0.253531546818095</v>
       </c>
       <c r="T14" s="0" t="n">
         <v>6.93369308589753</v>
       </c>
       <c r="U14" s="0" t="n">
         <f aca="false">((T14-6.6)/1.5)*$AH14</f>
-        <v>0.0375960876777887</v>
+        <v>0.0375960876777884</v>
       </c>
       <c r="V14" s="0" t="n">
         <f aca="false">((T14-$AF14)/$AG14)*$AH14</f>
-        <v>0.179609696891858</v>
+        <v>0.179609696891857</v>
       </c>
       <c r="W14" s="0" t="n">
         <v>6.77116226044188</v>
       </c>
       <c r="X14" s="0" t="n">
         <f aca="false">((W14-6.6)/1.5)*$AH14</f>
-        <v>0.0192842813431184</v>
+        <v>0.0192842813431185</v>
       </c>
       <c r="Y14" s="0" t="n">
         <f aca="false">((W14-$AF14)/$AG14)*$AH14</f>
@@ -3698,11 +3767,11 @@
       </c>
       <c r="AA14" s="0" t="n">
         <f aca="false">((Z14-6.6)/1.5)*$AH14</f>
-        <v>-0.015919756796606</v>
+        <v>-0.0159197567966056</v>
       </c>
       <c r="AB14" s="0" t="n">
         <f aca="false">((Z14-$AF14)/$AG14)*$AH14</f>
-        <v>0.0525991782093432</v>
+        <v>0.0525991782093438</v>
       </c>
       <c r="AC14" s="0" t="n">
         <v>5.48429086970795</v>
@@ -3721,7 +3790,7 @@
       </c>
       <c r="AG14" s="0" t="n">
         <f aca="false">STDEV(B14,E14,H14,K14,N14,Q14,T14,W14,Z14,AC14)</f>
-        <v>0.632024556267268</v>
+        <v>0.632024556267267</v>
       </c>
       <c r="AH14" s="0" t="n">
         <v>0.169</v>
@@ -3740,7 +3809,7 @@
       </c>
       <c r="D15" s="0" t="n">
         <f aca="false">((B15-AF15)/AG15)*$AH15</f>
-        <v>0.0778719547021565</v>
+        <v>0.0778719547021566</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>9.69715569076742</v>
@@ -3758,11 +3827,11 @@
       </c>
       <c r="I15" s="0" t="n">
         <f aca="false">((H15-2.1)/1.2)*$AH15</f>
-        <v>0.912663973097829</v>
+        <v>0.912663973097828</v>
       </c>
       <c r="J15" s="0" t="n">
         <f aca="false">((H15-$AF15)/$AG15)*$AH15</f>
-        <v>0.0391419912397991</v>
+        <v>0.0391419912397984</v>
       </c>
       <c r="K15" s="0" t="n">
         <v>6.16138151800337</v>
@@ -3773,7 +3842,7 @@
       </c>
       <c r="M15" s="0" t="n">
         <f aca="false">((K15-$AF15)/$AG15)*$AH15</f>
-        <v>-0.244202078753002</v>
+        <v>-0.244202078753001</v>
       </c>
       <c r="N15" s="0" t="n">
         <v>6.48683922251917</v>
@@ -3795,7 +3864,7 @@
       </c>
       <c r="S15" s="0" t="n">
         <f aca="false">((Q15-$AF15)/$AG15)*$AH15</f>
-        <v>-0.0868042895393009</v>
+        <v>-0.0868042895393012</v>
       </c>
       <c r="T15" s="0" t="n">
         <v>6.94404474418656</v>
@@ -3817,7 +3886,7 @@
       </c>
       <c r="Y15" s="0" t="n">
         <f aca="false">((W15-$AF15)/$AG15)*$AH15</f>
-        <v>-0.0975882550388409</v>
+        <v>-0.0975882550388418</v>
       </c>
       <c r="Z15" s="0" t="n">
         <v>9.38308402274812</v>
@@ -3843,7 +3912,7 @@
       </c>
       <c r="AF15" s="0" t="n">
         <f aca="false">AVERAGE(B15,E15,H15,K15,N15,Q15,T15,W15,Z15,AC15)</f>
-        <v>7.96387733693801</v>
+        <v>7.96387733693802</v>
       </c>
       <c r="AG15" s="0" t="n">
         <f aca="false">STDEV(B15,E15,H15,K15,N15,Q15,T15,W15,Z15,AC15)</f>
@@ -3974,11 +4043,11 @@
       </c>
       <c r="B21" s="0" t="n">
         <f aca="false">SUM(D2:D15)</f>
-        <v>0.589316093149846</v>
+        <v>0.589316093149854</v>
       </c>
       <c r="C21" s="0" t="n">
         <f aca="false">SUM(G2:G15)</f>
-        <v>0.769070938437075</v>
+        <v>0.769070938437071</v>
       </c>
       <c r="D21" s="0" t="n">
         <f aca="false">SUM(J2:J15)</f>
@@ -3986,31 +4055,31 @@
       </c>
       <c r="E21" s="0" t="n">
         <f aca="false">SUM(M2:M15)</f>
-        <v>-0.940274366354744</v>
+        <v>-0.940274366354746</v>
       </c>
       <c r="F21" s="0" t="n">
         <f aca="false">SUM(P2:P15)</f>
-        <v>-0.381046846971477</v>
+        <v>-0.381046846971482</v>
       </c>
       <c r="G21" s="0" t="n">
         <f aca="false">SUM(S2:S15)</f>
-        <v>-0.699813504438221</v>
+        <v>-0.699813504438222</v>
       </c>
       <c r="H21" s="0" t="n">
         <f aca="false">SUM(V2:V15)</f>
-        <v>0.319632873542753</v>
+        <v>0.319632873542751</v>
       </c>
       <c r="I21" s="0" t="n">
         <f aca="false">SUM(Y2:Y15)</f>
-        <v>0.71116187254442</v>
+        <v>0.711161872544419</v>
       </c>
       <c r="J21" s="0" t="n">
         <f aca="false">SUM(AB2:AB15)</f>
-        <v>0.414857460646138</v>
+        <v>0.414857460646142</v>
       </c>
       <c r="K21" s="0" t="n">
         <f aca="false">SUM(AE2:AE15)</f>
-        <v>-0.271455865108802</v>
+        <v>-0.271455865108803</v>
       </c>
       <c r="M21" s="0" t="s">
         <v>74</v>
@@ -4033,7 +4102,7 @@
       </c>
       <c r="D22" s="0" t="n">
         <f aca="false">(D21+D20)/2</f>
-        <v>0.64560843442506</v>
+        <v>0.645608434425059</v>
       </c>
       <c r="E22" s="0" t="n">
         <f aca="false">(E21+E20)/2</f>
@@ -4041,11 +4110,11 @@
       </c>
       <c r="F22" s="0" t="n">
         <f aca="false">(F21+F20)/2</f>
-        <v>0.67565509496187</v>
+        <v>0.675655094961867</v>
       </c>
       <c r="G22" s="0" t="n">
         <f aca="false">(G21+G20)/2</f>
-        <v>0.476102099642085</v>
+        <v>0.476102099642084</v>
       </c>
       <c r="H22" s="0" t="n">
         <f aca="false">(H21+H20)/2</f>
@@ -4053,11 +4122,11 @@
       </c>
       <c r="I22" s="0" t="n">
         <f aca="false">(I21+I20)/2</f>
-        <v>1.59988309358618</v>
+        <v>1.59988309358617</v>
       </c>
       <c r="J22" s="0" t="n">
         <f aca="false">(J21+J20)/2</f>
-        <v>1.40703479113063</v>
+        <v>1.40703479113064</v>
       </c>
       <c r="K22" s="0" t="n">
         <f aca="false">(K21+K20)/2</f>
@@ -4069,7 +4138,7 @@
       </c>
       <c r="N22" s="0" t="n">
         <f aca="false">STDEV(B22:K22)</f>
-        <v>0.527891300855015</v>
+        <v>0.527891300855016</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4099,7 +4168,7 @@
       </c>
       <c r="G23" s="0" t="n">
         <f aca="false">'lit values'!G16</f>
-        <v>0.200097009280448</v>
+        <v>0.200097009280447</v>
       </c>
       <c r="H23" s="0" t="n">
         <f aca="false">'lit values'!H16</f>
@@ -4609,10 +4678,10 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A4:K4 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -5206,4 +5275,763 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:Q7"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H1" activeCellId="1" sqref="A4:K4 H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" s="5" customFormat="true" ht="27.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>273</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:N20"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4:K4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>110</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>1250</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="N3" s="0" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>0.152</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>0.157</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>0.184</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>0.112</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>0.044</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>0.203</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>0.156</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>0.167</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>0.122</v>
+      </c>
+      <c r="M4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="N4" s="0" t="n">
+        <v>-0.129</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>0.035</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>0.038</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>0.037</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>0.039</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>0.044</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>0.019</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>0.013</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="M5" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="N5" s="0" t="n">
+        <v>-0.115</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>0.122</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>0.113</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>0.153</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>0.161</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>0.108</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>0.106</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>0.219</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>0.133</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>0.143</v>
+      </c>
+      <c r="M6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="N6" s="0" t="n">
+        <v>-0.102</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M7" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="N7" s="0" t="n">
+        <v>-0.099</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>0.096</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>0.096</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>0.095</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>0.102</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>0.072</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>0.084</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>0.056</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>0.038</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>0.082</v>
+      </c>
+      <c r="M8" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="N8" s="0" t="n">
+        <v>-0.044</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>0.148</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>0.111</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>0.076</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>0.102</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>0.078</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>0.081</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>0.038</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>0.087</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>0.143</v>
+      </c>
+      <c r="M9" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="N9" s="0" t="n">
+        <v>-0.043</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>0.107</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>0.133</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>0.205</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>0.133</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>0.133</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>0.156</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>0.178</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>0.269</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>0.204</v>
+      </c>
+      <c r="M10" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="N10" s="0" t="n">
+        <v>0.015</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>0.141</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>0.133</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>0.138</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>0.133</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>0.139</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>0.128</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>0.147</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <v>0.061</v>
+      </c>
+      <c r="M11" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="N11" s="0" t="n">
+        <v>0.065</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M12" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="N12" s="0" t="n">
+        <v>0.134</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>0.026</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>0.052</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>0.054</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>0.027</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>0.033</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>0.056</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <v>0.031</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>0.006</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <v>0.013</v>
+      </c>
+      <c r="K13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="N13" s="0" t="n">
+        <v>0.134</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>0.034</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>0.036</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>0.054</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>0.035</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>0.039</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <v>0.032</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <v>0.031</v>
+      </c>
+      <c r="J14" s="0" t="n">
+        <v>0.013</v>
+      </c>
+      <c r="K14" s="0" t="n">
+        <v>0.061</v>
+      </c>
+      <c r="M14" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="N14" s="0" t="n">
+        <v>0.139</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M15" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="N15" s="0" t="n">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>0.059</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>0.051</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>0.053</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>0.067</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <v>0.064</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <v>0.088</v>
+      </c>
+      <c r="I16" s="0" t="n">
+        <v>0.025</v>
+      </c>
+      <c r="J16" s="0" t="n">
+        <v>0.027</v>
+      </c>
+      <c r="K16" s="0" t="n">
+        <v>0.061</v>
+      </c>
+      <c r="M16" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="N16" s="0" t="n">
+        <v>0.169</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>0.018</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>0.018</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M17" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="N17" s="0" t="n">
+        <v>0.178</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>0.078</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" s="0" t="n">
+        <v>0.006</v>
+      </c>
+      <c r="J18" s="0" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="K18" s="0" t="n">
+        <v>0.041</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>0.044</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>0.049</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>0.104</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>0.089</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <v>0.076</v>
+      </c>
+      <c r="H19" s="0" t="n">
+        <v>0.031</v>
+      </c>
+      <c r="I19" s="0" t="n">
+        <v>0.013</v>
+      </c>
+      <c r="J19" s="0" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="K19" s="0" t="n">
+        <v>0.041</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>0.006</v>
+      </c>
+      <c r="I20" s="0" t="n">
+        <v>0.006</v>
+      </c>
+      <c r="J20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" s="0" t="n">
+        <v>0.02</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>